<commit_message>
Refinamiento de CA y prototipo
</commit_message>
<xml_diff>
--- a/Analisis/Epicas.xlsx
+++ b/Analisis/Epicas.xlsx
@@ -550,16 +550,16 @@
     <t>3.2 CA 2</t>
   </si>
   <si>
-    <t>Aplicación de descuentos</t>
-  </si>
-  <si>
-    <t>Que soy el administrador del sistema y haya configurado un descuento para la membresía</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Establezco el periodo de vigencia del descuento </t>
-  </si>
-  <si>
-    <t>El sistema deberá validar las fechas de inicio y fin de la suscripción. (PROTOTIPO #14)</t>
+    <t>Consulta de membresia</t>
+  </si>
+  <si>
+    <t>Que soy el administrador del sistema y haya entradp al modulo de membresía de clientes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cuando consulto el periodo de vigencia del descuento </t>
+  </si>
+  <si>
+    <t>El sistema deberá mostrar las fechas de inicio y fin de la suscripción. (PROTOTIPO #14)</t>
   </si>
   <si>
     <t>3.2 CA 3</t>
@@ -571,7 +571,7 @@
     <t>Que el sistema cuenta con un plan de membresías</t>
   </si>
   <si>
-    <t>Se establece un descuento para la adquisición o renovación de membresía</t>
+    <t>Se establece un descuento por defecto para la adquisición</t>
   </si>
   <si>
     <t>Se creará un porcentaje o monto fijo de descuento aplicable a la membresía. (PROTOTIPO #15)</t>
@@ -1006,14 +1006,14 @@
     <xf borderId="1" fillId="2" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment readingOrder="0"/>
+    </xf>
     <xf borderId="1" fillId="0" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="left" readingOrder="1" shrinkToFit="0" vertical="center" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="1" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment readingOrder="0"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="2" fillId="3" fontId="2" numFmtId="0" xfId="0" applyBorder="1" applyFill="1" applyFont="1"/>
@@ -1207,7 +1207,7 @@
     <xdr:ext cx="4791075" cy="3105150"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image17.png"/>
+        <xdr:cNvPr id="0" name="image9.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1235,7 +1235,7 @@
     <xdr:ext cx="4343400" cy="2838450"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Interfaz de usuario gráfica&#10;&#10;Descripción generada automáticamente" id="0" name="image5.png"/>
+        <xdr:cNvPr descr="Interfaz de usuario gráfica&#10;&#10;Descripción generada automáticamente" id="0" name="image18.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1263,7 +1263,7 @@
     <xdr:ext cx="4714875" cy="3038475"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Interfaz de usuario gráfica, Sitio web&#10;&#10;Descripción generada automáticamente" id="0" name="image1.png"/>
+        <xdr:cNvPr descr="Interfaz de usuario gráfica, Sitio web&#10;&#10;Descripción generada automáticamente" id="0" name="image13.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1291,7 +1291,7 @@
     <xdr:ext cx="4581525" cy="3067050"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image2.png"/>
+        <xdr:cNvPr id="0" name="image20.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1319,7 +1319,7 @@
     <xdr:ext cx="4800600" cy="3067050"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Interfaz de usuario gráfica, Calendario&#10;&#10;Descripción generada automáticamente" id="0" name="image4.png"/>
+        <xdr:cNvPr descr="Interfaz de usuario gráfica, Calendario&#10;&#10;Descripción generada automáticamente" id="0" name="image17.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1347,7 +1347,7 @@
     <xdr:ext cx="4772025" cy="3105150"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr descr="Interfaz de usuario gráfica&#10;&#10;Descripción generada automáticamente" id="0" name="image3.png"/>
+        <xdr:cNvPr descr="Interfaz de usuario gráfica&#10;&#10;Descripción generada automáticamente" id="0" name="image8.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1375,7 +1375,7 @@
     <xdr:ext cx="5067300" cy="3314700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image18.png"/>
+        <xdr:cNvPr id="0" name="image19.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1403,7 +1403,7 @@
     <xdr:ext cx="4914900" cy="3238500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image15.png"/>
+        <xdr:cNvPr id="0" name="image12.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1431,7 +1431,7 @@
     <xdr:ext cx="4848225" cy="3209925"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image6.png"/>
+        <xdr:cNvPr id="0" name="image10.png"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1459,7 +1459,7 @@
     <xdr:ext cx="4714875" cy="3362325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image9.jpg" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image6.jpg" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1487,7 +1487,7 @@
     <xdr:ext cx="4581525" cy="3362325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image13.jpg" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image15.jpg" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1543,7 +1543,7 @@
     <xdr:ext cx="4772025" cy="3314700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image12.jpg" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image11.jpg" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1571,7 +1571,7 @@
     <xdr:ext cx="4514850" cy="3314700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image14.jpg" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image16.jpg" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1599,7 +1599,7 @@
     <xdr:ext cx="4714875" cy="3314700"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image19.jpg" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image2.jpg" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1627,7 +1627,7 @@
     <xdr:ext cx="4772025" cy="3362325"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image8.jpg" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image5.jpg" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1655,7 +1655,7 @@
     <xdr:ext cx="4514850" cy="3238500"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image16.jpg" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image21.jpg" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1683,7 +1683,7 @@
     <xdr:ext cx="4848225" cy="3495675"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image10.jpg" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image14.jpg" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1711,7 +1711,7 @@
     <xdr:ext cx="4514850" cy="3495675"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image20.jpg" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image1.jpg" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -1731,15 +1731,43 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:ext cx="5838825" cy="4152900"/>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="0" name="image4.jpg" title="Imagen"/>
+        <xdr:cNvPicPr preferRelativeResize="0"/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip cstate="print" r:embed="rId17"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData fLocksWithSheet="0"/>
+  </xdr:oneCellAnchor>
+  <xdr:oneCellAnchor>
+    <xdr:from>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>866775</xdr:colOff>
+      <xdr:colOff>876300</xdr:colOff>
       <xdr:row>126</xdr:row>
       <xdr:rowOff>-200025</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="4914900" cy="3495675"/>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="0" name="image11.jpg" title="Imagen"/>
+        <xdr:cNvPr id="0" name="image3.jpg" title="Imagen"/>
         <xdr:cNvPicPr preferRelativeResize="0"/>
       </xdr:nvPicPr>
       <xdr:blipFill>
@@ -4574,7 +4602,7 @@
       <c r="C28" s="3" t="s">
         <v>120</v>
       </c>
-      <c r="D28" s="2" t="s">
+      <c r="D28" s="7" t="s">
         <v>121</v>
       </c>
       <c r="E28" s="2" t="s">
@@ -4585,13 +4613,13 @@
       </c>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="B29" s="2" t="s">
+      <c r="B29" s="7" t="s">
         <v>124</v>
       </c>
       <c r="C29" s="3" t="s">
         <v>125</v>
       </c>
-      <c r="D29" s="7" t="s">
+      <c r="D29" s="8" t="s">
         <v>121</v>
       </c>
       <c r="E29" s="2" t="s">
@@ -4602,7 +4630,7 @@
       </c>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="C30" s="8"/>
+      <c r="C30" s="9"/>
     </row>
     <row r="31" ht="15.75" customHeight="1"/>
     <row r="32" ht="15.75" customHeight="1">
@@ -4806,7 +4834,7 @@
       <c r="D47" s="3" t="s">
         <v>168</v>
       </c>
-      <c r="E47" s="9" t="s">
+      <c r="E47" s="7" t="s">
         <v>169</v>
       </c>
       <c r="F47" s="3" t="s">
@@ -4853,13 +4881,13 @@
       <c r="B52" s="2" t="s">
         <v>176</v>
       </c>
-      <c r="C52" s="3" t="s">
+      <c r="C52" s="5" t="s">
         <v>177</v>
       </c>
-      <c r="D52" s="3" t="s">
+      <c r="D52" s="5" t="s">
         <v>178</v>
       </c>
-      <c r="E52" s="3" t="s">
+      <c r="E52" s="5" t="s">
         <v>179</v>
       </c>
       <c r="F52" s="5" t="s">
@@ -4870,13 +4898,13 @@
       <c r="B53" s="2" t="s">
         <v>181</v>
       </c>
-      <c r="C53" s="3" t="s">
+      <c r="C53" s="5" t="s">
         <v>182</v>
       </c>
       <c r="D53" s="2" t="s">
         <v>183</v>
       </c>
-      <c r="E53" s="3" t="s">
+      <c r="E53" s="5" t="s">
         <v>184</v>
       </c>
       <c r="F53" s="5" t="s">
@@ -8418,7 +8446,7 @@
       <c r="D7" s="2" t="s">
         <v>268</v>
       </c>
-      <c r="E7" s="9" t="s">
+      <c r="E7" s="7" t="s">
         <v>269</v>
       </c>
     </row>
@@ -8429,7 +8457,7 @@
       <c r="C8" s="2" t="s">
         <v>271</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="7" t="s">
         <v>272</v>
       </c>
       <c r="E8" s="2" t="s">
@@ -8443,7 +8471,7 @@
       <c r="C9" s="2" t="s">
         <v>275</v>
       </c>
-      <c r="D9" s="9" t="s">
+      <c r="D9" s="7" t="s">
         <v>276</v>
       </c>
       <c r="E9" s="2" t="s">

</xml_diff>